<commit_message>
Updated the webhook file with strapi code
</commit_message>
<xml_diff>
--- a/documents/Review/API Reviews.xlsx
+++ b/documents/Review/API Reviews.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Beckn\ETS-Assembly-Python-Code\documents\Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9942D9-FA4D-458C-A6FA-2D1275FAD50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DFF90B-9B8F-46C3-9128-5738D29CAAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C1256C5C-4F35-42B0-8A8F-FE9AF9949CEA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C1256C5C-4F35-42B0-8A8F-FE9AF9949CEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Requests" sheetId="1" r:id="rId1"/>
@@ -494,7 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB51EC0-56A0-4500-812B-5E8F7B84D5F2}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -554,7 +554,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1BA6B5-B4CB-46FE-9F78-A66CF66A974F}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -643,7 +645,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F24D197A-2569-4C20-8CF0-C243DD67418B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>